<commit_message>
update 28 March 2019
</commit_message>
<xml_diff>
--- a/BOM/White Knight Documentation.xlsx
+++ b/BOM/White Knight Documentation.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Downloads\Da Vinci 3D printer\renders\Belt printer\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4ADC92-7C28-4206-B383-772D863B0B07}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5BE870-2B0B-41CD-A40B-FA495B9F1E36}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1A9839D0-F1F9-40EB-A8FA-A873B328377D}"/>
+    <workbookView xWindow="1446" yWindow="1362" windowWidth="10488" windowHeight="8994" activeTab="1" xr2:uid="{1A9839D0-F1F9-40EB-A8FA-A873B328377D}"/>
   </bookViews>
   <sheets>
     <sheet name="34pin connector" sheetId="1" r:id="rId1"/>
     <sheet name="BOM" sheetId="2" r:id="rId2"/>
-    <sheet name="Bulk Hardware" sheetId="3" r:id="rId3"/>
+    <sheet name="Extrusions" sheetId="4" r:id="rId3"/>
+    <sheet name="Bulk Hardware" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="160">
   <si>
     <t>Color</t>
   </si>
@@ -239,9 +240,6 @@
     <t>Rubber feet</t>
   </si>
   <si>
-    <t>1/2" 20.5" Stainless steel rod</t>
-  </si>
-  <si>
     <t>Noctua 40mm fans Qty 3</t>
   </si>
   <si>
@@ -477,6 +475,45 @@
   </si>
   <si>
     <t>Stainless Steel Round Bar 1/2" x 20.5"</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>4080 C-Channel</t>
+  </si>
+  <si>
+    <t>914mm</t>
+  </si>
+  <si>
+    <t>2040 V-slot</t>
+  </si>
+  <si>
+    <t>520mm</t>
+  </si>
+  <si>
+    <t>700mm</t>
+  </si>
+  <si>
+    <t>460mm</t>
+  </si>
+  <si>
+    <t>453mm</t>
+  </si>
+  <si>
+    <t>2020 V-slot</t>
+  </si>
+  <si>
+    <t>315mm</t>
+  </si>
+  <si>
+    <t>1/2" x 19" aluminum sqaure bar</t>
   </si>
 </sst>
 </file>
@@ -936,7 +973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C05BAE-1283-4F62-A89B-70F4991C7357}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -1296,11 +1333,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B27:B30"/>
     <mergeCell ref="B31:B32"/>
     <mergeCell ref="B33:B36"/>
     <mergeCell ref="B3:B4"/>
@@ -1309,6 +1341,11 @@
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B11:B14"/>
     <mergeCell ref="B15:B18"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1319,8 +1356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E665A9A7-D1EB-4ADF-AEF8-07F3A1E51DC0}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1335,11 +1372,11 @@
         <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G1" s="14">
         <f>SUM(B4:B203)</f>
-        <v>2255.8200000000002</v>
+        <v>1847.24</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1542,43 +1579,43 @@
         <v>57</v>
       </c>
       <c r="B20" s="14">
-        <v>21.21</v>
+        <v>24.68</v>
       </c>
       <c r="C20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B21" s="14">
         <v>50.64</v>
       </c>
       <c r="C21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B22" s="14">
         <v>34.32</v>
       </c>
       <c r="C22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B23" s="14">
         <v>19.28</v>
       </c>
       <c r="C23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -1589,7 +1626,7 @@
         <v>210</v>
       </c>
       <c r="C24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -1649,18 +1686,18 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>68</v>
+        <v>159</v>
       </c>
       <c r="B30" s="14">
-        <v>420</v>
+        <v>7.95</v>
       </c>
       <c r="C30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B31" s="14">
         <v>45</v>
@@ -1671,71 +1708,71 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B32" s="14">
         <v>12</v>
       </c>
       <c r="C32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B33" s="14">
         <v>6</v>
       </c>
       <c r="C33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B34" s="14">
         <v>50</v>
       </c>
       <c r="C34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B35" s="14">
         <v>18</v>
       </c>
       <c r="C35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B36" s="14">
         <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B37" s="14">
         <v>202.73</v>
       </c>
       <c r="C37" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1745,6 +1782,106 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9453373D-B946-4FB1-A78C-99B0BC673040}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="14.68359375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE808631-DED2-48D0-A77B-120E1872D02B}">
   <dimension ref="A1:D30"/>
   <sheetViews>
@@ -1761,301 +1898,301 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
         <v>80</v>
-      </c>
-      <c r="B1" t="s">
-        <v>81</v>
       </c>
       <c r="C1" t="s">
         <v>37</v>
       </c>
       <c r="D1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B2">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5">
         <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6">
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B9">
         <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B10">
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B12">
         <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B14">
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B16">
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B17">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B18">
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B19">
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B20">
         <v>118</v>
       </c>
       <c r="C20" t="s">
+        <v>139</v>
+      </c>
+      <c r="D20" t="s">
         <v>140</v>
-      </c>
-      <c r="D20" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B21">
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B22">
         <v>10</v>
@@ -2063,63 +2200,63 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B23">
         <v>104</v>
       </c>
       <c r="C23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B24">
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B25">
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B26">
         <v>18</v>
       </c>
       <c r="C26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -2127,7 +2264,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B28">
         <v>6</v>
@@ -2135,30 +2272,30 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B29">
         <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B30">
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D30" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update White Knight Documentation.xlsx
</commit_message>
<xml_diff>
--- a/BOM/White Knight Documentation.xlsx
+++ b/BOM/White Knight Documentation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Downloads\Da Vinci 3D printer\renders\Belt printer\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A34F661-7DF6-4B7D-A018-321CF3D27DFA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F66FCDA-E51D-48AF-8788-9E64AC7B1C91}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="834" yWindow="108" windowWidth="14754" windowHeight="11676" activeTab="1" xr2:uid="{1A9839D0-F1F9-40EB-A8FA-A873B328377D}"/>
+    <workbookView xWindow="2304" yWindow="1152" windowWidth="17280" windowHeight="9984" activeTab="1" xr2:uid="{1A9839D0-F1F9-40EB-A8FA-A873B328377D}"/>
   </bookViews>
   <sheets>
     <sheet name="34pin connector" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="179">
   <si>
     <t>Color</t>
   </si>
@@ -516,7 +516,61 @@
     <t>1/2" x 19" aluminum sqaure bar</t>
   </si>
   <si>
-    <t>TBD</t>
+    <t>Digikey.com</t>
+  </si>
+  <si>
+    <t>34 Pin Male IDC connector</t>
+  </si>
+  <si>
+    <t>TME.com</t>
+  </si>
+  <si>
+    <t>AWHP-34P</t>
+  </si>
+  <si>
+    <t>34 Pin Female IDC Connector</t>
+  </si>
+  <si>
+    <t>3M157228-ND</t>
+  </si>
+  <si>
+    <t>4 position Molex Plug</t>
+  </si>
+  <si>
+    <t>WM1018-ND</t>
+  </si>
+  <si>
+    <t>4 position Molex receptical</t>
+  </si>
+  <si>
+    <t>WM3701-ND</t>
+  </si>
+  <si>
+    <t>Molex Male pin</t>
+  </si>
+  <si>
+    <t>WM2500-ND</t>
+  </si>
+  <si>
+    <t>Molex female pin</t>
+  </si>
+  <si>
+    <t>WM2501-ND</t>
+  </si>
+  <si>
+    <t>20AWG 2 conductor blk/red</t>
+  </si>
+  <si>
+    <t>CN180BR-25-ND</t>
+  </si>
+  <si>
+    <t>26AWG 34 cond multi color ribbon</t>
+  </si>
+  <si>
+    <t>3M157870-25-ND</t>
+  </si>
+  <si>
+    <t>thebigbearingstore.com</t>
   </si>
 </sst>
 </file>
@@ -526,7 +580,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -542,8 +596,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF24292E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF24292E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -622,8 +689,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6F8FA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -631,11 +710,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDFE2E5"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDFE2E5"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDFE2E5"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDFE2E5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -651,10 +745,29 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -980,20 +1093,20 @@
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.68359375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.3125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1004,332 +1117,332 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="16"/>
+      <c r="B4" s="22"/>
       <c r="C4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="22" t="s">
         <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="16"/>
+      <c r="B6" s="22"/>
       <c r="C6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="22" t="s">
         <v>14</v>
       </c>
       <c r="C7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="16"/>
+      <c r="B8" s="22"/>
       <c r="C8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="22" t="s">
         <v>15</v>
       </c>
       <c r="C9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="16"/>
+      <c r="B10" s="22"/>
       <c r="C10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="22" t="s">
         <v>16</v>
       </c>
       <c r="C11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="16"/>
+      <c r="B12" s="22"/>
       <c r="C12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="16"/>
+      <c r="B13" s="22"/>
       <c r="C13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="16"/>
+      <c r="B14" s="22"/>
       <c r="C14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="22" t="s">
         <v>17</v>
       </c>
       <c r="C15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="16"/>
+      <c r="B16" s="22"/>
       <c r="C16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="16"/>
+      <c r="B17" s="22"/>
       <c r="C17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="16"/>
+      <c r="B18" s="22"/>
       <c r="C18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="22" t="s">
         <v>18</v>
       </c>
       <c r="C19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="16"/>
+      <c r="B20" s="22"/>
       <c r="C20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="16"/>
+      <c r="B21" s="22"/>
       <c r="C21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="16"/>
+      <c r="B22" s="22"/>
       <c r="C22" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="22" t="s">
         <v>19</v>
       </c>
       <c r="C23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="16"/>
+      <c r="B24" s="22"/>
       <c r="C24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="22" t="s">
         <v>20</v>
       </c>
       <c r="C25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="16"/>
+      <c r="B26" s="22"/>
       <c r="C26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="22" t="s">
         <v>21</v>
       </c>
       <c r="C27" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="16"/>
+      <c r="B28" s="22"/>
       <c r="C28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="16"/>
+      <c r="B29" s="22"/>
       <c r="C29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="16"/>
+      <c r="B30" s="22"/>
       <c r="C30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="21" t="s">
         <v>22</v>
       </c>
       <c r="C31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="15"/>
+      <c r="B32" s="21"/>
       <c r="C32" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="21" t="s">
         <v>23</v>
       </c>
       <c r="C33" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B34" s="15"/>
+      <c r="B34" s="21"/>
       <c r="C34" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B35" s="15"/>
+      <c r="B35" s="21"/>
       <c r="C35" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="15"/>
+      <c r="B36" s="21"/>
       <c r="C36" t="s">
         <v>30</v>
       </c>
@@ -1357,20 +1470,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E665A9A7-D1EB-4ADF-AEF8-07F3A1E51DC0}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.89453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.83984375" style="14"/>
-    <col min="3" max="3" width="20.26171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="14"/>
+    <col min="3" max="3" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -1378,11 +1492,11 @@
         <v>76</v>
       </c>
       <c r="G1" s="14">
-        <f>SUM(B4:B203)</f>
-        <v>1697.24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <f>SUM(B4:B202)</f>
+        <v>2036.78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -1393,7 +1507,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>61</v>
       </c>
@@ -1404,7 +1518,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1415,7 +1529,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1426,7 +1540,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -1437,7 +1551,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -1448,7 +1562,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -1459,7 +1573,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -1470,7 +1584,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -1481,7 +1595,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -1492,7 +1606,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -1503,7 +1617,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -1514,7 +1628,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -1525,7 +1639,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -1536,7 +1650,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -1547,7 +1661,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -1558,15 +1672,18 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>55</v>
       </c>
       <c r="B18" s="14">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>11</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -1577,7 +1694,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -1588,7 +1705,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>144</v>
       </c>
@@ -1599,7 +1716,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>145</v>
       </c>
@@ -1610,7 +1727,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>146</v>
       </c>
@@ -1621,7 +1738,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>58</v>
       </c>
@@ -1632,18 +1749,18 @@
         <v>141</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="14" t="s">
-        <v>160</v>
+      <c r="B25" s="14">
+        <v>290</v>
       </c>
       <c r="C25" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>63</v>
       </c>
@@ -1654,7 +1771,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -1665,7 +1782,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>66</v>
       </c>
@@ -1676,7 +1793,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>67</v>
       </c>
@@ -1687,7 +1804,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>159</v>
       </c>
@@ -1698,7 +1815,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>68</v>
       </c>
@@ -1709,7 +1826,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>69</v>
       </c>
@@ -1720,7 +1837,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>71</v>
       </c>
@@ -1731,7 +1848,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>73</v>
       </c>
@@ -1742,7 +1859,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>74</v>
       </c>
@@ -1753,7 +1870,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>75</v>
       </c>
@@ -1764,7 +1881,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>137</v>
       </c>
@@ -1776,6 +1893,118 @@
       </c>
       <c r="D37" t="s">
         <v>143</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B38" s="19">
+        <v>1.32</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="B39" s="20">
+        <v>1.38</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="B40" s="19">
+        <v>0.36</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="B41" s="20">
+        <v>0.31</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="B42" s="19">
+        <v>1.68</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="B43" s="20">
+        <v>1.7</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="B44" s="19">
+        <v>19.54</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="B45" s="20">
+        <v>50.25</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -1792,17 +2021,17 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.68359375" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>147</v>
       </c>
@@ -1813,7 +2042,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>150</v>
       </c>
@@ -1824,7 +2053,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>152</v>
       </c>
@@ -1835,7 +2064,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>152</v>
       </c>
@@ -1846,7 +2075,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>152</v>
       </c>
@@ -1857,7 +2086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>152</v>
       </c>
@@ -1868,7 +2097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>157</v>
       </c>
@@ -1892,14 +2121,14 @@
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.47265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.83984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.26171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>79</v>
       </c>
@@ -1913,7 +2142,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -1927,7 +2156,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>83</v>
       </c>
@@ -1941,7 +2170,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -1955,7 +2184,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -1969,7 +2198,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>86</v>
       </c>
@@ -1983,7 +2212,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>88</v>
       </c>
@@ -1997,7 +2226,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>87</v>
       </c>
@@ -2011,7 +2240,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>89</v>
       </c>
@@ -2025,7 +2254,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>90</v>
       </c>
@@ -2039,7 +2268,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>91</v>
       </c>
@@ -2053,7 +2282,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>92</v>
       </c>
@@ -2067,7 +2296,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>93</v>
       </c>
@@ -2081,7 +2310,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>94</v>
       </c>
@@ -2095,7 +2324,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>95</v>
       </c>
@@ -2109,7 +2338,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>96</v>
       </c>
@@ -2123,7 +2352,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>97</v>
       </c>
@@ -2137,7 +2366,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>98</v>
       </c>
@@ -2151,7 +2380,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -2165,7 +2394,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>100</v>
       </c>
@@ -2179,7 +2408,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>101</v>
       </c>
@@ -2193,7 +2422,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>102</v>
       </c>
@@ -2201,7 +2430,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>108</v>
       </c>
@@ -2215,7 +2444,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>103</v>
       </c>
@@ -2229,7 +2458,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>107</v>
       </c>
@@ -2243,7 +2472,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>111</v>
       </c>
@@ -2257,7 +2486,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>104</v>
       </c>
@@ -2265,7 +2494,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>105</v>
       </c>
@@ -2273,7 +2502,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>116</v>
       </c>
@@ -2287,7 +2516,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>118</v>
       </c>

</xml_diff>